<commit_message>
added a field to change the name of the saved xlsx
</commit_message>
<xml_diff>
--- a/resources/rdv_base.xlsx
+++ b/resources/rdv_base.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="10"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="capa" sheetId="1" state="visible" r:id="rId2"/>
@@ -483,7 +483,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="3" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="5" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -589,9 +589,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>456480</xdr:colOff>
+      <xdr:colOff>456120</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>408960</xdr:rowOff>
+      <xdr:rowOff>408600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -604,8 +604,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="257040" y="123840"/>
-          <a:ext cx="1541160" cy="285120"/>
+          <a:off x="276120" y="123840"/>
+          <a:ext cx="1713240" cy="284760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -626,9 +626,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>208800</xdr:colOff>
+      <xdr:colOff>208440</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>37080</xdr:rowOff>
+      <xdr:rowOff>36720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -641,8 +641,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9410760" y="19080"/>
-          <a:ext cx="3052800" cy="551160"/>
+          <a:off x="10374840" y="19080"/>
+          <a:ext cx="3839040" cy="550800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -668,9 +668,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>56520</xdr:colOff>
+      <xdr:colOff>56160</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>342360</xdr:rowOff>
+      <xdr:rowOff>342000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -684,7 +684,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="209520" y="76320"/>
-          <a:ext cx="2119320" cy="266040"/>
+          <a:ext cx="2444400" cy="265680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -705,9 +705,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>1534680</xdr:colOff>
+      <xdr:colOff>1534320</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>46800</xdr:rowOff>
+      <xdr:rowOff>46440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -720,8 +720,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10495080" y="0"/>
-          <a:ext cx="1477440" cy="492480"/>
+          <a:off x="11984760" y="0"/>
+          <a:ext cx="1477080" cy="492120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -747,9 +747,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>56520</xdr:colOff>
+      <xdr:colOff>56160</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>342360</xdr:rowOff>
+      <xdr:rowOff>342000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -763,7 +763,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="209520" y="76320"/>
-          <a:ext cx="2119320" cy="266040"/>
+          <a:ext cx="2444400" cy="265680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -784,9 +784,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>1534680</xdr:colOff>
+      <xdr:colOff>1534320</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>46800</xdr:rowOff>
+      <xdr:rowOff>46440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -799,8 +799,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10495080" y="0"/>
-          <a:ext cx="1477440" cy="492480"/>
+          <a:off x="11984760" y="0"/>
+          <a:ext cx="1477080" cy="492120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -826,9 +826,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>56520</xdr:colOff>
+      <xdr:colOff>56160</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>342360</xdr:rowOff>
+      <xdr:rowOff>342000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -842,7 +842,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="209520" y="76320"/>
-          <a:ext cx="2119320" cy="266040"/>
+          <a:ext cx="2444400" cy="265680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -863,9 +863,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>1534680</xdr:colOff>
+      <xdr:colOff>1534320</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>46800</xdr:rowOff>
+      <xdr:rowOff>46440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -878,8 +878,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10495080" y="0"/>
-          <a:ext cx="1477440" cy="492480"/>
+          <a:off x="11984760" y="0"/>
+          <a:ext cx="1477080" cy="492120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -905,9 +905,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>56520</xdr:colOff>
+      <xdr:colOff>56160</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>342360</xdr:rowOff>
+      <xdr:rowOff>342000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -921,7 +921,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="209520" y="76320"/>
-          <a:ext cx="2119320" cy="266040"/>
+          <a:ext cx="2444400" cy="265680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -942,9 +942,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>1534680</xdr:colOff>
+      <xdr:colOff>1534320</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>46800</xdr:rowOff>
+      <xdr:rowOff>46440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -957,8 +957,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10495080" y="0"/>
-          <a:ext cx="1477440" cy="492480"/>
+          <a:off x="11984760" y="0"/>
+          <a:ext cx="1477080" cy="492120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -984,9 +984,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>56520</xdr:colOff>
+      <xdr:colOff>56160</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>342360</xdr:rowOff>
+      <xdr:rowOff>342000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1000,7 +1000,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="209520" y="76320"/>
-          <a:ext cx="2119320" cy="266040"/>
+          <a:ext cx="2444400" cy="265680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1021,9 +1021,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>1534680</xdr:colOff>
+      <xdr:colOff>1534320</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>46800</xdr:rowOff>
+      <xdr:rowOff>46440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1036,8 +1036,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10495080" y="0"/>
-          <a:ext cx="1477440" cy="492480"/>
+          <a:off x="11984760" y="0"/>
+          <a:ext cx="1477080" cy="492120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1063,9 +1063,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>56520</xdr:colOff>
+      <xdr:colOff>56160</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>342360</xdr:rowOff>
+      <xdr:rowOff>342000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1079,7 +1079,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="209520" y="76320"/>
-          <a:ext cx="2119320" cy="266040"/>
+          <a:ext cx="2444400" cy="265680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1100,9 +1100,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>1534680</xdr:colOff>
+      <xdr:colOff>1534320</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>46800</xdr:rowOff>
+      <xdr:rowOff>46440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1115,8 +1115,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10495080" y="0"/>
-          <a:ext cx="1477440" cy="492480"/>
+          <a:off x="11984760" y="0"/>
+          <a:ext cx="1477080" cy="492120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1142,9 +1142,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>56520</xdr:colOff>
+      <xdr:colOff>56160</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>342360</xdr:rowOff>
+      <xdr:rowOff>342000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1158,7 +1158,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="209520" y="76320"/>
-          <a:ext cx="2119320" cy="266040"/>
+          <a:ext cx="2444400" cy="265680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1179,9 +1179,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>1534680</xdr:colOff>
+      <xdr:colOff>1534320</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>46800</xdr:rowOff>
+      <xdr:rowOff>46440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1194,8 +1194,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10495080" y="0"/>
-          <a:ext cx="1477440" cy="492480"/>
+          <a:off x="11984760" y="0"/>
+          <a:ext cx="1477080" cy="492120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1221,9 +1221,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>56520</xdr:colOff>
+      <xdr:colOff>56160</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>342360</xdr:rowOff>
+      <xdr:rowOff>342000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1237,7 +1237,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="209520" y="76320"/>
-          <a:ext cx="2119320" cy="266040"/>
+          <a:ext cx="2444400" cy="265680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1258,9 +1258,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>1534680</xdr:colOff>
+      <xdr:colOff>1534320</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>46800</xdr:rowOff>
+      <xdr:rowOff>46440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1273,8 +1273,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10495080" y="0"/>
-          <a:ext cx="1477440" cy="492480"/>
+          <a:off x="11984760" y="0"/>
+          <a:ext cx="1477080" cy="492120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1300,9 +1300,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>56520</xdr:colOff>
+      <xdr:colOff>56160</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>342360</xdr:rowOff>
+      <xdr:rowOff>342000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1316,7 +1316,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="209520" y="76320"/>
-          <a:ext cx="2119320" cy="266040"/>
+          <a:ext cx="2444400" cy="265680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1337,9 +1337,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>1534680</xdr:colOff>
+      <xdr:colOff>1534320</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>46800</xdr:rowOff>
+      <xdr:rowOff>46440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1352,8 +1352,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10495080" y="0"/>
-          <a:ext cx="1477440" cy="492480"/>
+          <a:off x="11984760" y="0"/>
+          <a:ext cx="1477080" cy="492120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1379,9 +1379,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>56520</xdr:colOff>
+      <xdr:colOff>56160</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>342360</xdr:rowOff>
+      <xdr:rowOff>342000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1395,7 +1395,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="209520" y="76320"/>
-          <a:ext cx="2119320" cy="266040"/>
+          <a:ext cx="2444400" cy="265680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1416,9 +1416,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>1534680</xdr:colOff>
+      <xdr:colOff>1534320</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>46800</xdr:rowOff>
+      <xdr:rowOff>46440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1431,8 +1431,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10495080" y="0"/>
-          <a:ext cx="1477440" cy="492480"/>
+          <a:off x="11984760" y="0"/>
+          <a:ext cx="1477080" cy="492120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1454,20 +1454,20 @@
   </sheetPr>
   <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I11" activeCellId="0" sqref="I11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G20" activeCellId="0" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="1.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="3" style="1" width="11.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="16.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="16.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="7.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="66.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="1" width="11.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="2.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="3" style="1" width="13.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="18.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="19.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="8.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="75.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="1" width="13.6"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="42" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1660,7 +1660,7 @@
       <c r="E20" s="24"/>
       <c r="F20" s="24"/>
       <c r="G20" s="25" t="n">
-        <f aca="false">(verso1!I24)</f>
+        <f aca="false">(verso0!I24+verso1!I24+verso2!I24+verso3!I24+verso4!I24+verso5!I24+verso6!I24+verso7!I24+verso8!I24+verso9!I24)</f>
         <v>0</v>
       </c>
     </row>
@@ -1702,7 +1702,7 @@
     <row r="24" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B24" s="26" t="n">
         <f aca="true">TODAY()</f>
-        <v>43281</v>
+        <v>43282</v>
       </c>
       <c r="C24" s="26"/>
       <c r="D24" s="20"/>
@@ -1787,7 +1787,7 @@
   <pageSetup paperSize="9" scale="98" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
-    <oddFooter>&amp;R&amp;"Sans,Regular"Sans,Regular" 83679603-FIP-BRA-PT-002</oddFooter>
+    <oddFooter>&amp;R&amp;"Sans,Regular"Sans,Regular"Sans,Regular" 83679603-FIP-BRA-PT-002</oddFooter>
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -1806,11 +1806,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="21.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="3" style="1" width="16.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="32.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="1" width="11.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="24.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="3" style="1" width="18.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="37.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="1" width="13.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="35.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2205,7 +2205,7 @@
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
-    <oddFooter>&amp;R&amp;"Sans,Regular"Sans,Regular" 83679603-FIP-BRA-PT-001</oddFooter>
+    <oddFooter>&amp;R&amp;"Sans,Regular"Sans,Regular"Sans,Regular" 83679603-FIP-BRA-PT-001</oddFooter>
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -2218,17 +2218,17 @@
   </sheetPr>
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="21.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="3" style="1" width="16.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="32.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="1" width="11.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="24.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="3" style="1" width="18.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="37.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="1" width="13.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="35.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2623,7 +2623,7 @@
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
-    <oddFooter>&amp;R&amp;"Sans,Regular"Sans,Regular" 83679603-FIP-BRA-PT-001</oddFooter>
+    <oddFooter>&amp;R&amp;"Sans,Regular"Sans,Regular"Sans,Regular" 83679603-FIP-BRA-PT-001</oddFooter>
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -2636,17 +2636,17 @@
   </sheetPr>
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="21.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="3" style="1" width="16.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="32.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="1" width="11.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="24.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="3" style="1" width="18.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="37.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="1" width="13.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="35.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3041,7 +3041,7 @@
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
-    <oddFooter>&amp;R&amp;"Sans,Regular"Sans,Regular" 83679603-FIP-BRA-PT-001</oddFooter>
+    <oddFooter>&amp;R&amp;"Sans,Regular"Sans,Regular"Sans,Regular" 83679603-FIP-BRA-PT-001</oddFooter>
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -3060,11 +3060,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="21.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="3" style="1" width="16.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="32.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="1" width="11.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="24.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="3" style="1" width="18.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="37.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="1" width="13.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="35.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3459,7 +3459,7 @@
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
-    <oddFooter>&amp;R&amp;"Sans,Regular"Sans,Regular" 83679603-FIP-BRA-PT-001</oddFooter>
+    <oddFooter>&amp;R&amp;"Sans,Regular"Sans,Regular"Sans,Regular" 83679603-FIP-BRA-PT-001</oddFooter>
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -3478,11 +3478,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="21.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="3" style="1" width="16.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="32.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="1" width="11.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="24.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="3" style="1" width="18.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="37.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="1" width="13.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="35.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3877,7 +3877,7 @@
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
-    <oddFooter>&amp;R&amp;"Sans,Regular"Sans,Regular" 83679603-FIP-BRA-PT-001</oddFooter>
+    <oddFooter>&amp;R&amp;"Sans,Regular"Sans,Regular"Sans,Regular" 83679603-FIP-BRA-PT-001</oddFooter>
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -3890,17 +3890,17 @@
   </sheetPr>
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="21.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="3" style="1" width="16.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="32.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="1" width="11.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="24.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="3" style="1" width="18.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="37.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="1" width="13.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="35.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4295,7 +4295,7 @@
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
-    <oddFooter>&amp;R&amp;"Sans,Regular"Sans,Regular" 83679603-FIP-BRA-PT-001</oddFooter>
+    <oddFooter>&amp;R&amp;"Sans,Regular"Sans,Regular"Sans,Regular" 83679603-FIP-BRA-PT-001</oddFooter>
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -4314,11 +4314,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="21.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="3" style="1" width="16.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="32.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="1" width="11.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="24.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="3" style="1" width="18.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="37.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="1" width="13.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="35.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4713,7 +4713,7 @@
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
-    <oddFooter>&amp;R&amp;"Sans,Regular"Sans,Regular" 83679603-FIP-BRA-PT-001</oddFooter>
+    <oddFooter>&amp;R&amp;"Sans,Regular"Sans,Regular"Sans,Regular" 83679603-FIP-BRA-PT-001</oddFooter>
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -4732,11 +4732,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="21.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="3" style="1" width="16.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="32.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="1" width="11.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="24.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="3" style="1" width="18.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="37.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="1" width="13.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="35.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5131,7 +5131,7 @@
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
-    <oddFooter>&amp;R&amp;"Sans,Regular"Sans,Regular" 83679603-FIP-BRA-PT-001</oddFooter>
+    <oddFooter>&amp;R&amp;"Sans,Regular"Sans,Regular"Sans,Regular" 83679603-FIP-BRA-PT-001</oddFooter>
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -5150,11 +5150,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="21.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="3" style="1" width="16.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="32.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="1" width="11.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="24.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="3" style="1" width="18.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="37.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="1" width="13.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="35.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5549,7 +5549,7 @@
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
-    <oddFooter>&amp;R&amp;"Sans,Regular"Sans,Regular" 83679603-FIP-BRA-PT-001</oddFooter>
+    <oddFooter>&amp;R&amp;"Sans,Regular"Sans,Regular"Sans,Regular" 83679603-FIP-BRA-PT-001</oddFooter>
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -5568,11 +5568,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="21.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="3" style="1" width="16.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="32.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="1" width="11.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="24.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="3" style="1" width="18.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="37.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="1" width="13.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="35.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5967,7 +5967,7 @@
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
-    <oddFooter>&amp;R&amp;"Sans,Regular"Sans,Regular" 83679603-FIP-BRA-PT-001</oddFooter>
+    <oddFooter>&amp;R&amp;"Sans,Regular"Sans,Regular"Sans,Regular" 83679603-FIP-BRA-PT-001</oddFooter>
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>